<commit_message>
Corrige arquivo Excel com formato real .xlsx
</commit_message>
<xml_diff>
--- a/data/base_de_dados.xlsx
+++ b/data/base_de_dados.xlsx
@@ -29,10 +29,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Segoe UI"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">no caso de PTH esse campo é relacionado a placa
 </t>
@@ -168,11 +168,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -188,12 +189,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -238,12 +233,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,170 +271,170 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="28.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>45966</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>9248</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>45967</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>8289</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="1"/>
+      <c r="R3" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Adiciona rotina de atualização automática da base e integra auto_updater.py
</commit_message>
<xml_diff>
--- a/data/base_de_dados.xlsx
+++ b/data/base_de_dados.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="130">
   <si>
     <t xml:space="preserve">DATA</t>
   </si>
@@ -109,6 +109,9 @@
     <t xml:space="preserve">AF</t>
   </si>
   <si>
+    <t xml:space="preserve">AF1</t>
+  </si>
+  <si>
     <t xml:space="preserve">CARLOS</t>
   </si>
   <si>
@@ -127,9 +130,6 @@
     <t xml:space="preserve">CORTADO</t>
   </si>
   <si>
-    <t xml:space="preserve">DEZEMBRO</t>
-  </si>
-  <si>
     <t xml:space="preserve">2°</t>
   </si>
   <si>
@@ -158,6 +158,282 @@
   </si>
   <si>
     <t xml:space="preserve">LCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUGUSTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RISCADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUEBRADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUEDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTRAGEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2º</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AF3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DANIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOM ALTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TORTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5615-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALEX PORTILHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NÃO LIGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUPORTE MICRO CHAVE P60D17L-D4 127V 21L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICRO CHAVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABERTO (A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NÃO DA SOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJUSTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4899-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOSÉ NEPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEM AUDIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COND C CNX 7P 300MM USB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABO 7V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAU CONTATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5504-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANDERSON REIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEM SINAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOLHA POLARIZADORA 0.285M 90°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOLHA POLARIZADORA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTAMINAÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8832-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEYLA SAMANTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEM LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCI PRINCIPAL-FONTE KTC 32 ANDROID LG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EM ANÁLISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM-606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFGH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEM BOBINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2555-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFGDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THIAGO LEAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC PRINCIPAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTERADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SGF</t>
   </si>
 </sst>
 </file>
@@ -263,10 +539,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -352,25 +628,25 @@
         <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="1" t="n">
         <v>1</v>
@@ -387,10 +663,10 @@
         <v>45967</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>28</v>
@@ -435,6 +711,543 @@
         <v>30</v>
       </c>
       <c r="R3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>45968</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>45969</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>5413</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>45970</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>4164</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>45971</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>45972</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>45973</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>45974</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>45975</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>45976</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>45977</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="R13" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>